<commit_message>
Update VERA - Referentiedata - 2021-09-24.xlsx
</commit_message>
<xml_diff>
--- a/Referentiedata/VERA - Referentiedata - 2021-09-24.xlsx
+++ b/Referentiedata/VERA - Referentiedata - 2021-09-24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martijn\AppData\Local\GitHubDesktop\app-2.9.0\VERA\VERA-Standaard\Referentiedata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4386D480-065D-43E2-A656-27E28CA48C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232E9C8C-FD5E-435D-B143-2A9C77C0FF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2235" windowWidth="21600" windowHeight="11385" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VERA referentiedata" sheetId="14" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6934" uniqueCount="3733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6935" uniqueCount="3734">
   <si>
     <t>Referentiedatasoort</t>
   </si>
@@ -11286,6 +11286,9 @@
   </si>
   <si>
     <t>PASSENDHEIDSSOORT.NIE </t>
+  </si>
+  <si>
+    <t>..</t>
   </si>
 </sst>
 </file>
@@ -11990,8 +11993,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27388343-0A0E-446E-86B4-9C4356EB993E}" name="Tabel1" displayName="Tabel1" ref="A1:K1046" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:K1046" xr:uid="{8B075628-E833-48DC-8779-68AB54AC5BC1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27388343-0A0E-446E-86B4-9C4356EB993E}" name="Tabel1" displayName="Tabel1" ref="A1:K1047" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:K1047" xr:uid="{8B075628-E833-48DC-8779-68AB54AC5BC1}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{845F9FC6-EA7E-42C8-9954-6B75834B5282}" name="Referentiedatasoort" dataDxfId="19"/>
     <tableColumn id="7" xr3:uid="{ABFA2115-257A-4C72-8D5D-B12F03C0BC13}" name="Sortering" dataDxfId="18"/>
@@ -12363,10 +12366,10 @@
   <sheetPr codeName="Blad1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L1046"/>
+  <dimension ref="A1:L1047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1038" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1046" sqref="A1046"/>
+    <sheetView tabSelected="1" topLeftCell="A1035" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1048" sqref="A1048"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34233,6 +34236,21 @@
         <v>3732</v>
       </c>
       <c r="K1046" s="50"/>
+    </row>
+    <row r="1047" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1047" s="10" t="s">
+        <v>3733</v>
+      </c>
+      <c r="B1047" s="10"/>
+      <c r="C1047" s="10"/>
+      <c r="D1047" s="11"/>
+      <c r="E1047" s="11"/>
+      <c r="F1047" s="11"/>
+      <c r="G1047" s="11"/>
+      <c r="H1047" s="10"/>
+      <c r="I1047" s="10"/>
+      <c r="J1047" s="10"/>
+      <c r="K1047" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -40477,21 +40495,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFD438D9B9ABE14A977C2E01E1E997E9" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="238b4f00df057bc2742cc7aff66473ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="41b44f4d-acd5-45c0-8ca7-9032ca64d707" xmlns:ns3="bc2bfcf0-0204-42b7-916d-bc08fc5e6372" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfb8db5c6f5549a83cd0326992bdc891" ns2:_="" ns3:_="">
     <xsd:import namespace="41b44f4d-acd5-45c0-8ca7-9032ca64d707"/>
@@ -40694,24 +40697,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E3AA29B-E85A-4662-AF70-E41EEBB4502A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6EB239C-D482-4083-A20F-2310AB45B47F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9FCA9DB-B654-4D97-A1BC-1B4528FD4E25}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -40728,4 +40729,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6EB239C-D482-4083-A20F-2310AB45B47F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E3AA29B-E85A-4662-AF70-E41EEBB4502A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>